<commit_message>
Updated script to handle column mappings and empty data
</commit_message>
<xml_diff>
--- a/Input/Weekly_Template.xlsx
+++ b/Input/Weekly_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80f9cc67cdd945d7/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthik/Documents/Python Automation/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A263EB05-6911-3949-A0D5-C1E495F49B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B89EFF-B940-A946-ADB5-6014E64381FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112994D0-2AD3-3948-AD1F-B47C2FD3028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" xr2:uid="{CD633FF6-3351-AC48-9B9F-93271281531A}"/>
   </bookViews>
@@ -36,75 +36,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Opportunity Amount</t>
-  </si>
-  <si>
-    <t>Stage</t>
-  </si>
-  <si>
-    <t>Owner Name</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Created Date</t>
   </si>
   <si>
-    <t>Last Modified Date</t>
-  </si>
-  <si>
     <t>SFID</t>
   </si>
   <si>
-    <t>SF12345</t>
-  </si>
-  <si>
-    <t>ABC Corp</t>
-  </si>
-  <si>
-    <t>Qualified</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>SF67890</t>
-  </si>
-  <si>
-    <t>XYZ Inc.</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>SF98765</t>
-  </si>
-  <si>
-    <t>DEF Ltd.</t>
-  </si>
-  <si>
-    <t>Prospect</t>
-  </si>
-  <si>
-    <t>Mike Johnson</t>
-  </si>
-  <si>
-    <t>Asia</t>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>Opportunity Description</t>
+  </si>
+  <si>
+    <t>Group SBU</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Proposed Sub. Date</t>
+  </si>
+  <si>
+    <t>Domain Practice</t>
+  </si>
+  <si>
+    <t>Tech Practice</t>
+  </si>
+  <si>
+    <t>Solution SPOCs</t>
+  </si>
+  <si>
+    <t>Delivery SPOC</t>
+  </si>
+  <si>
+    <t>Proposal Owner</t>
+  </si>
+  <si>
+    <t>Proposal Writer</t>
+  </si>
+  <si>
+    <t>Orals SPOC</t>
+  </si>
+  <si>
+    <t>Bid Director</t>
+  </si>
+  <si>
+    <t>Proposal Updates</t>
+  </si>
+  <si>
+    <t>Proposal Status</t>
+  </si>
+  <si>
+    <t>Actual Sub. Date</t>
+  </si>
+  <si>
+    <t>Commercial Value</t>
+  </si>
+  <si>
+    <t>DSC</t>
+  </si>
+  <si>
+    <t>Opportunity Stage</t>
+  </si>
+  <si>
+    <t>Post Sub. Activity</t>
+  </si>
+  <si>
+    <t>Est. Deal Value</t>
+  </si>
+  <si>
+    <t>Large Deal</t>
   </si>
 </sst>
 </file>
@@ -175,10 +181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,117 +500,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D3EF8-C43E-DD43-B081-AD411B034FE0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3">
-        <v>44927</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45056</v>
-      </c>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2">
-        <v>250000</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3">
-        <v>44972</v>
-      </c>
-      <c r="H3" s="3">
-        <v>45061</v>
-      </c>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2">
-        <v>50000</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45005</v>
-      </c>
-      <c r="H4" s="3">
-        <v>45078</v>
-      </c>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>